<commit_message>
Create new functions CREATE DATABASE AND CLOSE DRIVERS
</commit_message>
<xml_diff>
--- a/parser/database.xlsx
+++ b/parser/database.xlsx
@@ -413,14 +413,1215 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Возьму собаку до года маленьких пород</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Возьму собаку до года маленьких пород</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>б-р Космонавтов, 38</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Отдам взрослую чихуашку</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5 000 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Отдам взрослую чихуашку</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Мусинская ул., 42</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Колобочки- сыночки, в добрые ручки</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ул. Калинина</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Колобочки- сыночки, в добрые ручки</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>б-р Космонавтов</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>8 000 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Амстаф</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Амстаф</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ул. Калинина</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ул. Островского</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ул. Калинина</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Джейси</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Джейси</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ул. Калинина, 90</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Щенки английского кокер спаниеля</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ул. Калинина, 90</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Щенки английского кокер спаниеля</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ленинградская ул.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Собака- Чапа</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ул. Калинина</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Собака- Чапа</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>7 500 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Линда</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Линда</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ул. Новаторов, 7</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Щенок в добрые руки</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Щенок в добрые руки</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ул. Ленина, 7/18</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Рада</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Рада</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1 000 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Собака- Гретта</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Собака- Гретта</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>б-р Монтажников</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Марта-собака стерилизована</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Марта-собака стерилизована</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Уфимская ул., 96</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3 000 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Линда-собачка стерилизована</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ул. Калинина, 43</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Линда-собачка стерилизована</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Питбуль Вязка</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>10 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Питбуль Вязка</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, городской округ Салават</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2 000 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Марта</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ул. Бочкарёва, 9А</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Марта</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Уфимская ул.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Сибирский хаски</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Сибирский хаски</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Чудесный щенок</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>10 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Чудесный щенок</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Щенки шпица</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Щенки шпица</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Вязка</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ул. Островского, 46</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Вязка</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ул. Ленина, 41</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Отдам щенка</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>д. Верхнеюлдашево, ул. Агидель, 21А</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Отдам щенка</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Щенята</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Щенята</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Центральная пл. имени В.И. Ленина</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Хаски для вязки. Кобель</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ул. Горького</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>100 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Хаски для вязки. Кобель</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Революционная ул., 3</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Бесплатно</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Чудесный щенок ищет дом</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Республика Башкортостан, Салават</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>50 ₽</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Чудесный щенок ищет дом</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ул. Калинина, 53</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Цена не указана</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Щенки</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Щенки</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Аляскинский маламут</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Аляскинский маламут</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Щеночки в добрые руки</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Щеночки в добрые руки</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Очаровательный щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Очаровательный щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Йоркширский терьерВязка</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Йоркширский терьерВязка</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Ищем сучку для немецкого шпица(кабель ) вязка</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Ищем сучку для немецкого шпица(кабель ) вязка</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Помесь хаски</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Помесь хаски</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Ищем невесту корс</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Ищем невесту корс</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Отдам собаку</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Отдам собаку</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Бельгийская овчарка</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Бельгийская овчарка</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Собака в добрые руки щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Собака в добрые руки щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Собака(мальчик)</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Собака(мальчик)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Йоркширский терьер</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Йоркширский терьер</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Русский охотничий спаниель</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Русский охотничий спаниель</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Собака</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Щенок</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>